<commit_message>
support for multiple sheets in same excel
version2 with update for multiple worksheets in the same excel.
</commit_message>
<xml_diff>
--- a/all_excels_dir/user_list1.xlsx
+++ b/all_excels_dir/user_list1.xlsx
@@ -5,22 +5,24 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\sureshg\merge_excel2\parent\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\sureshg\merge_excel_files_with_different_column_names\all_excels_dir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6EF0457-3C4F-44E6-9006-7AB32C199120}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8428179-A9C2-43CC-9A02-24BA7EBC3C00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39900" yWindow="2175" windowWidth="17355" windowHeight="11805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30510" yWindow="1710" windowWidth="11610" windowHeight="11265" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="list1_sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="list2_sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="list3_sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
   <si>
     <t>First Name</t>
   </si>
@@ -89,6 +91,54 @@
   </si>
   <si>
     <t>suresh@gmail.com</t>
+  </si>
+  <si>
+    <t>Macy</t>
+  </si>
+  <si>
+    <t>Barker</t>
+  </si>
+  <si>
+    <t>macy@gmail.com</t>
+  </si>
+  <si>
+    <t>Casper</t>
+  </si>
+  <si>
+    <t>Pitts</t>
+  </si>
+  <si>
+    <t>casper@gmail.com</t>
+  </si>
+  <si>
+    <t>Seattle</t>
+  </si>
+  <si>
+    <t>New Jersey</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>Phoenix</t>
+  </si>
+  <si>
+    <t>Aleena</t>
+  </si>
+  <si>
+    <t>Cobb</t>
+  </si>
+  <si>
+    <t>Murray</t>
+  </si>
+  <si>
+    <t>Smart</t>
+  </si>
+  <si>
+    <t>aleena@gmail.com</t>
+  </si>
+  <si>
+    <t>murray@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -486,7 +536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -594,4 +644,172 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{622D09F3-F288-4FF2-B34E-EACF1BA44E30}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.36328125" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" customWidth="1"/>
+    <col min="3" max="3" width="21.6328125" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C5" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{15F1C8FA-69A1-45CF-B663-CD1F69992749}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{B13FFC01-63C7-41DB-8764-9AE16495E011}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9DD0B0C-5D83-4877-A61B-C01C0247783F}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.36328125" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" customWidth="1"/>
+    <col min="3" max="3" width="21.6328125" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C5" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{23DDC0B6-274F-46D7-A3B5-0DE0A3D25FA2}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{C6C0EC5E-2E31-4964-B92E-354D61853E79}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>